<commit_message>
corrections in template and vignette
- removed TODAY und USCHEDULED from the template
- removed TODAY from vignette and explained how
  (un)scheduled is deterimed automatically
</commit_message>
<xml_diff>
--- a/inst/template/projects.xlsx
+++ b/inst/template/projects.xlsx
@@ -11,8 +11,8 @@
     <sheet name="kitchen" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kitchen!$A$1:$N$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kitchen!$A$1:$N$9</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kitchen!$A$1:$N$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">kitchen!$A$1:$N$6</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t xml:space="preserve">section</t>
   </si>
@@ -69,12 +69,6 @@
   </si>
   <si>
     <t xml:space="preserve">0_prep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TODAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unscheduled</t>
   </si>
   <si>
     <t xml:space="preserve">I</t>
@@ -286,19 +280,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.58"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="41.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -352,22 +342,18 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="K2" s="5" t="n">
         <v>0</v>
@@ -381,10 +367,10 @@
         <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
@@ -392,14 +378,12 @@
       <c r="G3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="H3" s="5"/>
       <c r="I3" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K3" s="5" t="n">
         <v>0</v>
@@ -408,47 +392,45 @@
       <c r="M3" s="5"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" s="7" customFormat="true" ht="45.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="7" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5" t="s">
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="AMJ4" s="0"/>
-    </row>
-    <row r="5" s="7" customFormat="true" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
@@ -456,14 +438,12 @@
       <c r="G5" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K5" s="5" t="n">
         <v>0</v>
@@ -474,13 +454,13 @@
     </row>
     <row r="6" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
@@ -488,14 +468,12 @@
       <c r="G6" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K6" s="5" t="n">
         <v>0</v>
@@ -506,13 +484,13 @@
     </row>
     <row r="7" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
@@ -520,14 +498,12 @@
       <c r="G7" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K7" s="5" t="n">
         <v>0</v>
@@ -538,11 +514,11 @@
     </row>
     <row r="8" s="7" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
@@ -550,31 +526,29 @@
       <c r="G8" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="H8" s="5"/>
       <c r="I8" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K8" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" s="7" customFormat="true" ht="57.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="7" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
@@ -584,26 +558,24 @@
       <c r="G9" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="H9" s="5"/>
       <c r="I9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K9" s="5" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AMJ9" s="0"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N6"/>
+  <autoFilter ref="A1:N9"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>